<commit_message>
Added Ecommerce app test case at home
</commit_message>
<xml_diff>
--- a/MobileAppFramework/TestData/TestData.xlsx
+++ b/MobileAppFramework/TestData/TestData.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stale\git\mobileframework\MobileAppFramework\TestData\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F258C26E-6576-4591-92FF-4F493BEC161F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="23256" windowHeight="13176" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="FrenchMappings" sheetId="38" state="hidden" r:id="rId1"/>
@@ -33,9 +27,9 @@
     <definedName name="ToBeExecuted">Dropdowns!$D$2:$D$3</definedName>
     <definedName name="version">Dropdowns!$E$2:$E$7</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="124519"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -49,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1915" uniqueCount="823">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1922" uniqueCount="825">
   <si>
     <t>Module</t>
   </si>
@@ -2632,11 +2626,17 @@
   <si>
     <t>WifiName</t>
   </si>
+  <si>
+    <t>testProductNavigation</t>
+  </si>
+  <si>
+    <t>Store</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fonts count="8">
     <font>
       <sz val="11"/>
@@ -2808,61 +2808,6 @@
 
 <file path=xl/activeX/activeX1.xml><?xml version="1.0" encoding="utf-8"?>
 <ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{5512D116-5CC6-11CF-8D67-00AA00BDCE1D}" ax:persistence="persistStream" r:id="rId1"/>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>1</xdr:col>
-          <xdr:colOff>5701748</xdr:colOff>
-          <xdr:row>313</xdr:row>
-          <xdr:rowOff>119270</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>2</xdr:col>
-          <xdr:colOff>290305</xdr:colOff>
-          <xdr:row>315</xdr:row>
-          <xdr:rowOff>43070</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="34817" name="Control 1" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s34817"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001880000}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln w="9525">
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a:ln>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3154,26 +3099,26 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:D386"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="85.5703125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="85.5546875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="85.5703125" style="9"/>
-    <col min="3" max="3" width="162.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="85.5703125" style="9"/>
+    <col min="1" max="1" width="22.44140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="85.5546875" style="9"/>
+    <col min="3" max="3" width="162.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="85.5546875" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -3726,7 +3671,7 @@
         <v>744</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="30">
+    <row r="39" spans="1:4" ht="28.8">
       <c r="A39" s="9" t="s">
         <v>13</v>
       </c>
@@ -3808,7 +3753,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="30">
+    <row r="45" spans="1:4">
       <c r="A45" s="9" t="s">
         <v>156</v>
       </c>
@@ -3951,7 +3896,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="30">
+    <row r="58" spans="1:4" ht="28.8">
       <c r="A58" s="9" t="s">
         <v>156</v>
       </c>
@@ -4070,7 +4015,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="30">
+    <row r="67" spans="1:4" ht="28.8">
       <c r="A67" s="9" t="s">
         <v>156</v>
       </c>
@@ -4085,7 +4030,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="45">
+    <row r="68" spans="1:4" ht="28.8">
       <c r="A68" s="9" t="s">
         <v>156</v>
       </c>
@@ -4250,7 +4195,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:4" ht="30">
+    <row r="79" spans="1:4" ht="28.8">
       <c r="A79" s="9" t="s">
         <v>156</v>
       </c>
@@ -4310,7 +4255,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:4" ht="30">
+    <row r="83" spans="1:4" ht="28.8">
       <c r="A83" s="9" t="s">
         <v>156</v>
       </c>
@@ -4325,7 +4270,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:4" ht="30">
+    <row r="84" spans="1:4" ht="28.8">
       <c r="A84" s="9" t="s">
         <v>156</v>
       </c>
@@ -4340,7 +4285,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:4" ht="18">
+    <row r="85" spans="1:4" ht="17.399999999999999">
       <c r="A85" s="9" t="s">
         <v>334</v>
       </c>
@@ -4362,7 +4307,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="87" spans="1:4" ht="18">
+    <row r="87" spans="1:4" ht="17.399999999999999">
       <c r="A87" s="9" t="s">
         <v>334</v>
       </c>
@@ -4384,7 +4329,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="89" spans="1:4" ht="18">
+    <row r="89" spans="1:4" ht="17.399999999999999">
       <c r="A89" s="9" t="s">
         <v>334</v>
       </c>
@@ -4395,7 +4340,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="90" spans="1:4" ht="18">
+    <row r="90" spans="1:4" ht="17.399999999999999">
       <c r="A90" s="9" t="s">
         <v>334</v>
       </c>
@@ -4406,7 +4351,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="91" spans="1:4" ht="18">
+    <row r="91" spans="1:4" ht="17.399999999999999">
       <c r="A91" s="9" t="s">
         <v>334</v>
       </c>
@@ -4604,7 +4549,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="109" spans="1:4" ht="30">
+    <row r="109" spans="1:4" ht="28.8">
       <c r="A109" s="9" t="s">
         <v>334</v>
       </c>
@@ -4615,7 +4560,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="110" spans="1:4" ht="30">
+    <row r="110" spans="1:4" ht="28.8">
       <c r="A110" s="9" t="s">
         <v>334</v>
       </c>
@@ -4637,7 +4582,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="112" spans="1:4" ht="30">
+    <row r="112" spans="1:4">
       <c r="A112" s="9" t="s">
         <v>334</v>
       </c>
@@ -5492,7 +5437,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="169" spans="1:4" ht="30">
+    <row r="169" spans="1:4" ht="28.8">
       <c r="A169" s="9" t="s">
         <v>365</v>
       </c>
@@ -5522,7 +5467,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="171" spans="1:4" ht="30">
+    <row r="171" spans="1:4">
       <c r="A171" s="9" t="s">
         <v>365</v>
       </c>
@@ -5537,7 +5482,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="172" spans="1:4" ht="30">
+    <row r="172" spans="1:4" ht="28.8">
       <c r="A172" s="9" t="s">
         <v>365</v>
       </c>
@@ -5747,7 +5692,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="186" spans="1:4" ht="30">
+    <row r="186" spans="1:4" ht="28.8">
       <c r="A186" s="9" t="s">
         <v>145</v>
       </c>
@@ -5792,7 +5737,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="189" spans="1:4" ht="45">
+    <row r="189" spans="1:4" ht="28.8">
       <c r="A189" s="9" t="s">
         <v>145</v>
       </c>
@@ -5807,7 +5752,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="190" spans="1:4" ht="30">
+    <row r="190" spans="1:4" ht="28.8">
       <c r="A190" s="9" t="s">
         <v>145</v>
       </c>
@@ -5822,7 +5767,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="191" spans="1:4" ht="30">
+    <row r="191" spans="1:4" ht="28.8">
       <c r="A191" s="9" t="s">
         <v>145</v>
       </c>
@@ -5837,7 +5782,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="192" spans="1:4" ht="30">
+    <row r="192" spans="1:4" ht="28.8">
       <c r="A192" s="9" t="s">
         <v>145</v>
       </c>
@@ -5852,7 +5797,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="193" spans="1:4" ht="30">
+    <row r="193" spans="1:4" ht="28.8">
       <c r="A193" s="9" t="s">
         <v>145</v>
       </c>
@@ -5867,7 +5812,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="194" spans="1:4" ht="30">
+    <row r="194" spans="1:4" ht="28.8">
       <c r="A194" s="9" t="s">
         <v>145</v>
       </c>
@@ -5912,7 +5857,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="197" spans="1:4" ht="45">
+    <row r="197" spans="1:4" ht="28.8">
       <c r="A197" s="9" t="s">
         <v>145</v>
       </c>
@@ -5927,7 +5872,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="198" spans="1:4" ht="45">
+    <row r="198" spans="1:4" ht="28.8">
       <c r="A198" s="9" t="s">
         <v>145</v>
       </c>
@@ -5972,7 +5917,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="201" spans="1:4" ht="16.899999999999999" customHeight="1">
+    <row r="201" spans="1:4" ht="16.95" customHeight="1">
       <c r="A201" s="9" t="s">
         <v>145</v>
       </c>
@@ -6182,7 +6127,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="215" spans="1:4" ht="30">
+    <row r="215" spans="1:4" ht="28.8">
       <c r="A215" s="9" t="s">
         <v>6</v>
       </c>
@@ -6377,7 +6322,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="228" spans="1:4" ht="30">
+    <row r="228" spans="1:4" ht="28.8">
       <c r="A228" s="9" t="s">
         <v>321</v>
       </c>
@@ -6542,7 +6487,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="239" spans="1:4" ht="30">
+    <row r="239" spans="1:4" ht="28.8">
       <c r="A239" s="11" t="s">
         <v>367</v>
       </c>
@@ -7007,7 +6952,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="270" spans="1:4" ht="30">
+    <row r="270" spans="1:4" ht="28.8">
       <c r="A270" s="9" t="s">
         <v>547</v>
       </c>
@@ -7142,7 +7087,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="279" spans="1:4" ht="30">
+    <row r="279" spans="1:4" ht="28.8">
       <c r="A279" s="9" t="s">
         <v>14</v>
       </c>
@@ -7727,7 +7672,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="318" spans="1:4" ht="30">
+    <row r="318" spans="1:4" ht="28.8">
       <c r="A318" s="9" t="s">
         <v>14</v>
       </c>
@@ -7757,7 +7702,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="320" spans="1:4" ht="60">
+    <row r="320" spans="1:4" ht="43.2">
       <c r="A320" s="9" t="s">
         <v>14</v>
       </c>
@@ -7937,7 +7882,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="332" spans="1:4" ht="30">
+    <row r="332" spans="1:4">
       <c r="A332" s="9" t="s">
         <v>14</v>
       </c>
@@ -8297,7 +8242,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="356" spans="1:4" ht="30">
+    <row r="356" spans="1:4" ht="28.8">
       <c r="A356" s="9" t="s">
         <v>138</v>
       </c>
@@ -8312,7 +8257,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="357" spans="1:4" ht="30">
+    <row r="357" spans="1:4" ht="28.8">
       <c r="A357" s="9" t="s">
         <v>138</v>
       </c>
@@ -8387,7 +8332,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="362" spans="1:4" ht="30">
+    <row r="362" spans="1:4" ht="28.8">
       <c r="A362" s="9" t="s">
         <v>138</v>
       </c>
@@ -8738,61 +8683,36 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D372" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:D372"/>
   <hyperlinks>
-    <hyperlink ref="B236" r:id="rId1" display="https://qa2.wmcanada.com/ca/en/terms" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B199" r:id="rId2" display="https://www.wm.com/paymybill" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="C199" r:id="rId3" display="https://www.wm.com/paymybill" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="C342" r:id="rId4" display="https://support.wmcanada.com/hc/fr-ca/articles/360000994391" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B236" r:id="rId1" display="https://qa2.wmcanada.com/ca/en/terms"/>
+    <hyperlink ref="B199" r:id="rId2" display="https://www.wm.com/paymybill"/>
+    <hyperlink ref="C199" r:id="rId3" display="https://www.wm.com/paymybill"/>
+    <hyperlink ref="C342" r:id="rId4" display="https://support.wmcanada.com/hc/fr-ca/articles/360000994391"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId5"/>
-  <drawing r:id="rId6"/>
-  <legacyDrawing r:id="rId7"/>
+  <legacyDrawing r:id="rId6"/>
   <controls>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="34817" r:id="rId8" name="Control 1">
-          <controlPr defaultSize="0" r:id="rId9">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>313</xdr:row>
-                <xdr:rowOff>123825</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>285750</xdr:colOff>
-                <xdr:row>315</xdr:row>
-                <xdr:rowOff>47625</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="34817" r:id="rId8" name="Control 1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
+    <control shapeId="34817" r:id="rId7" name="Control 1"/>
   </controls>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet21"/>
   <dimension ref="A1:D140"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="85.5703125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="85.5546875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="84.28515625" style="9" customWidth="1"/>
-    <col min="3" max="3" width="85.5703125" style="9"/>
-    <col min="4" max="4" width="2.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="85.5703125" style="9"/>
+    <col min="1" max="1" width="22.44140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="84.33203125" style="9" customWidth="1"/>
+    <col min="3" max="3" width="85.5546875" style="9"/>
+    <col min="4" max="4" width="2.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="85.5546875" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -9316,7 +9236,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="45">
+    <row r="36" spans="1:4" ht="28.8">
       <c r="A36" s="9" t="s">
         <v>156</v>
       </c>
@@ -9331,7 +9251,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="45">
+    <row r="37" spans="1:4" ht="43.2">
       <c r="A37" s="9" t="s">
         <v>156</v>
       </c>
@@ -9496,7 +9416,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="30">
+    <row r="48" spans="1:4" ht="28.8">
       <c r="A48" s="9" t="s">
         <v>156</v>
       </c>
@@ -9571,7 +9491,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="45">
+    <row r="53" spans="1:4" ht="43.2">
       <c r="A53" s="9" t="s">
         <v>156</v>
       </c>
@@ -9586,7 +9506,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="30">
+    <row r="54" spans="1:4" ht="28.8">
       <c r="A54" s="9" t="s">
         <v>156</v>
       </c>
@@ -9598,7 +9518,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="30">
+    <row r="55" spans="1:4" ht="28.8">
       <c r="A55" s="9" t="s">
         <v>334</v>
       </c>
@@ -10288,7 +10208,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:4" ht="30">
+    <row r="101" spans="1:4" ht="28.8">
       <c r="A101" s="9" t="s">
         <v>145</v>
       </c>
@@ -10303,7 +10223,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:4" ht="30">
+    <row r="102" spans="1:4" ht="28.8">
       <c r="A102" s="9" t="s">
         <v>145</v>
       </c>
@@ -10318,7 +10238,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:4" ht="30">
+    <row r="103" spans="1:4">
       <c r="A103" s="9" t="s">
         <v>145</v>
       </c>
@@ -10333,7 +10253,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:4" ht="45">
+    <row r="104" spans="1:4" ht="43.2">
       <c r="A104" s="9" t="s">
         <v>145</v>
       </c>
@@ -10348,7 +10268,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:4" ht="30">
+    <row r="105" spans="1:4" ht="28.8">
       <c r="A105" s="9" t="s">
         <v>145</v>
       </c>
@@ -10363,7 +10283,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:4" ht="30">
+    <row r="106" spans="1:4" ht="28.8">
       <c r="A106" s="9" t="s">
         <v>145</v>
       </c>
@@ -10378,7 +10298,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:4" ht="30">
+    <row r="107" spans="1:4" ht="28.8">
       <c r="A107" s="9" t="s">
         <v>145</v>
       </c>
@@ -10393,7 +10313,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:4" ht="30">
+    <row r="108" spans="1:4" ht="28.8">
       <c r="A108" s="9" t="s">
         <v>145</v>
       </c>
@@ -10408,7 +10328,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:4" ht="30">
+    <row r="109" spans="1:4" ht="28.8">
       <c r="A109" s="9" t="s">
         <v>145</v>
       </c>
@@ -10453,7 +10373,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:4" ht="45">
+    <row r="112" spans="1:4" ht="43.2">
       <c r="A112" s="9" t="s">
         <v>145</v>
       </c>
@@ -10468,7 +10388,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:4" ht="45">
+    <row r="113" spans="1:4" ht="43.2">
       <c r="A113" s="9" t="s">
         <v>145</v>
       </c>
@@ -10483,7 +10403,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:4" ht="30">
+    <row r="114" spans="1:4">
       <c r="A114" s="9" t="s">
         <v>145</v>
       </c>
@@ -10498,7 +10418,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:4" ht="30">
+    <row r="115" spans="1:4">
       <c r="A115" s="9" t="s">
         <v>145</v>
       </c>
@@ -10753,7 +10673,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:4" ht="30">
+    <row r="132" spans="1:4" ht="28.8">
       <c r="A132" s="9" t="s">
         <v>321</v>
       </c>
@@ -10798,7 +10718,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:4" ht="30">
+    <row r="135" spans="1:4">
       <c r="A135" s="9" t="s">
         <v>145</v>
       </c>
@@ -10853,36 +10773,36 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D140" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
+  <autoFilter ref="A1:D140"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet33"/>
-  <dimension ref="A1:V5"/>
+  <dimension ref="A1:V6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="D5" sqref="D5"/>
       <selection pane="topRight" activeCell="D5" sqref="D5"/>
       <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
-      <selection pane="bottomRight" activeCell="C3" sqref="C3"/>
+      <selection pane="bottomRight" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.42578125" defaultRowHeight="18.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="16.44140625" defaultRowHeight="18.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" style="20" customWidth="1"/>
-    <col min="2" max="2" width="31.28515625" style="20" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" style="22" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" style="22"/>
-    <col min="5" max="5" width="19.140625" style="22" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="16.42578125" style="22"/>
-    <col min="8" max="8" width="13.5703125" style="22" customWidth="1"/>
-    <col min="9" max="22" width="10.7109375" style="22" customWidth="1"/>
-    <col min="23" max="16384" width="16.42578125" style="22"/>
+    <col min="1" max="1" width="16.88671875" style="20" customWidth="1"/>
+    <col min="2" max="2" width="31.33203125" style="20" customWidth="1"/>
+    <col min="3" max="3" width="14.5546875" style="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.44140625" style="22"/>
+    <col min="5" max="5" width="19.109375" style="22" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="16.44140625" style="22"/>
+    <col min="8" max="8" width="13.5546875" style="22" customWidth="1"/>
+    <col min="9" max="22" width="10.6640625" style="22" customWidth="1"/>
+    <col min="23" max="16384" width="16.44140625" style="22"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="18.75" customHeight="1">
@@ -11045,24 +10965,47 @@
         <v>796</v>
       </c>
     </row>
+    <row r="6" spans="1:22" ht="18.75" customHeight="1">
+      <c r="A6" s="20" t="s">
+        <v>824</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>823</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="22" t="s">
+        <v>797</v>
+      </c>
+      <c r="E6" s="22" t="s">
+        <v>104</v>
+      </c>
+      <c r="F6" s="22" t="s">
+        <v>816</v>
+      </c>
+      <c r="H6" s="24" t="s">
+        <v>796</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:V4" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
+  <autoFilter ref="A1:V4"/>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E5" xr:uid="{00000000-0002-0000-0200-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E6">
       <formula1>INDIRECT("Browsers_Devices")</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C5" xr:uid="{00000000-0002-0000-0200-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C6">
       <formula1>INDIRECT("ToBeExecuted")</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D5" xr:uid="{00000000-0002-0000-0200-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D6">
       <formula1>INDIRECT("Test_Platform")</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F5" xr:uid="{4F4627D7-F0B0-45CB-8BFC-38829ECDF492}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F6">
       <formula1>INDIRECT("version")</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="B2" location="testAutoPayEnrollment!A2" display="testAutoPayEnrollment" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="B2" location="testAutoPayEnrollment!A2" display="testAutoPayEnrollment"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -11070,20 +11013,20 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="34.28515625" style="16" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" style="16" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" style="16" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="16"/>
+    <col min="1" max="1" width="34.33203125" style="16" customWidth="1"/>
+    <col min="2" max="2" width="15.5546875" style="16" customWidth="1"/>
+    <col min="3" max="3" width="16.88671875" style="16" customWidth="1"/>
+    <col min="4" max="16384" width="9.109375" style="16"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="18" customFormat="1" ht="30" customHeight="1">
@@ -11108,7 +11051,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="30">
+    <row r="3" spans="1:3" ht="28.8">
       <c r="A3" s="16" t="s">
         <v>806</v>
       </c>
@@ -11119,7 +11062,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="30">
+    <row r="4" spans="1:3" ht="28.8">
       <c r="A4" s="16" t="s">
         <v>807</v>
       </c>
@@ -11130,7 +11073,7 @@
         <v>808</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="30">
+    <row r="5" spans="1:3" ht="28.8">
       <c r="A5" s="16" t="s">
         <v>811</v>
       </c>
@@ -11141,7 +11084,7 @@
         <v>809</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="30">
+    <row r="6" spans="1:3" ht="28.8">
       <c r="A6" s="16" t="s">
         <v>812</v>
       </c>
@@ -11154,7 +11097,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" location="TestCases!B6" display="Test Description" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="A1" location="TestCases!B6" display="Test Description"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -11162,7 +11105,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet17"/>
   <dimension ref="A1:R7"/>
   <sheetViews>
@@ -11174,25 +11117,25 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="19.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="19.6640625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="2" width="26.140625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="19.7109375" style="15"/>
-    <col min="4" max="6" width="26.140625" style="15" customWidth="1"/>
-    <col min="7" max="7" width="19.42578125" style="15" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.28515625" style="15" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.85546875" style="15" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.85546875" style="15" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.5703125" style="15" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.140625" style="15" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="26.109375" style="5" customWidth="1"/>
+    <col min="3" max="3" width="19.6640625" style="15"/>
+    <col min="4" max="6" width="26.109375" style="15" customWidth="1"/>
+    <col min="7" max="7" width="19.44140625" style="15" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.33203125" style="15" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.88671875" style="15" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.88671875" style="15" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.5546875" style="15" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.109375" style="15" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="20" style="15" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.7109375" style="15" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.140625" style="15" customWidth="1"/>
-    <col min="16" max="16" width="15.5703125" style="15" customWidth="1"/>
-    <col min="17" max="16384" width="19.7109375" style="15"/>
+    <col min="14" max="14" width="15.6640625" style="15" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.109375" style="15" customWidth="1"/>
+    <col min="16" max="16" width="15.5546875" style="15" customWidth="1"/>
+    <col min="17" max="16384" width="19.6640625" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="75">
+    <row r="1" spans="1:18" ht="57.6">
       <c r="A1" s="4" t="s">
         <v>38</v>
       </c>
@@ -11248,7 +11191,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="60">
+    <row r="2" spans="1:18" ht="57.6">
       <c r="A2" s="5" t="s">
         <v>743</v>
       </c>
@@ -11296,7 +11239,7 @@
       </c>
       <c r="R2" s="5"/>
     </row>
-    <row r="3" spans="1:18" ht="75">
+    <row r="3" spans="1:18" ht="57.6">
       <c r="A3" s="5" t="s">
         <v>724</v>
       </c>
@@ -11342,7 +11285,7 @@
       </c>
       <c r="R3" s="5"/>
     </row>
-    <row r="4" spans="1:18" ht="75">
+    <row r="4" spans="1:18" ht="57.6">
       <c r="A4" s="5" t="s">
         <v>722</v>
       </c>
@@ -11388,7 +11331,7 @@
       </c>
       <c r="R4" s="5"/>
     </row>
-    <row r="5" spans="1:18" ht="90">
+    <row r="5" spans="1:18" ht="72">
       <c r="A5" s="5" t="s">
         <v>721</v>
       </c>
@@ -11437,7 +11380,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="45">
+    <row r="6" spans="1:18" ht="28.8">
       <c r="A6" s="5" t="s">
         <v>370</v>
       </c>
@@ -11484,7 +11427,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="45">
+    <row r="7" spans="1:18" ht="43.2">
       <c r="A7" s="5" t="s">
         <v>725</v>
       </c>
@@ -11534,7 +11477,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" location="TestCases!B51" display="Test Description" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink ref="A1" location="TestCases!B51" display="Test Description"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -11542,7 +11485,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet18"/>
   <dimension ref="A1:S11"/>
   <sheetViews>
@@ -11554,28 +11497,28 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="19.7109375" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="19.6640625" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="2" width="26.140625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" style="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.42578125" style="15" customWidth="1"/>
-    <col min="5" max="7" width="26.140625" style="15" customWidth="1"/>
-    <col min="8" max="8" width="13.5703125" style="15" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.140625" style="15" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.42578125" style="15" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.28515625" style="15" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.85546875" style="15" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.85546875" style="15" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.5703125" style="15" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.140625" style="15" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="21.28515625" style="15" customWidth="1"/>
-    <col min="17" max="17" width="16.28515625" style="15" customWidth="1"/>
-    <col min="18" max="18" width="25.28515625" style="15" customWidth="1"/>
-    <col min="19" max="19" width="26.7109375" style="15" customWidth="1"/>
-    <col min="20" max="16384" width="19.7109375" style="15"/>
+    <col min="1" max="2" width="26.109375" style="5" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" style="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.44140625" style="15" customWidth="1"/>
+    <col min="5" max="7" width="26.109375" style="15" customWidth="1"/>
+    <col min="8" max="8" width="13.5546875" style="15" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.109375" style="15" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.44140625" style="15" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.33203125" style="15" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.88671875" style="15" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.88671875" style="15" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.5546875" style="15" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.109375" style="15" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21.33203125" style="15" customWidth="1"/>
+    <col min="17" max="17" width="16.33203125" style="15" customWidth="1"/>
+    <col min="18" max="18" width="25.33203125" style="15" customWidth="1"/>
+    <col min="19" max="19" width="26.6640625" style="15" customWidth="1"/>
+    <col min="20" max="16384" width="19.6640625" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="60">
+    <row r="1" spans="1:19" ht="57.6">
       <c r="A1" s="4" t="s">
         <v>38</v>
       </c>
@@ -11634,7 +11577,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="30">
+    <row r="2" spans="1:19" ht="28.8">
       <c r="A2" s="5" t="s">
         <v>88</v>
       </c>
@@ -11665,7 +11608,7 @@
       <c r="R2" s="3"/>
       <c r="S2" s="3"/>
     </row>
-    <row r="3" spans="1:19" ht="30">
+    <row r="3" spans="1:19" ht="28.8">
       <c r="A3" s="5" t="s">
         <v>90</v>
       </c>
@@ -11695,7 +11638,7 @@
       <c r="Q3" s="3"/>
       <c r="R3" s="3"/>
     </row>
-    <row r="4" spans="1:19" ht="30">
+    <row r="4" spans="1:19" ht="28.8">
       <c r="A4" s="5" t="s">
         <v>91</v>
       </c>
@@ -11725,7 +11668,7 @@
       <c r="Q4" s="3"/>
       <c r="R4" s="3"/>
     </row>
-    <row r="5" spans="1:19" ht="60">
+    <row r="5" spans="1:19" ht="43.2">
       <c r="A5" s="5" t="s">
         <v>741</v>
       </c>
@@ -11774,7 +11717,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="30">
+    <row r="6" spans="1:19" ht="28.8">
       <c r="A6" s="5" t="s">
         <v>723</v>
       </c>
@@ -11819,7 +11762,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="90">
+    <row r="7" spans="1:19" ht="72">
       <c r="A7" s="5" t="s">
         <v>125</v>
       </c>
@@ -11851,7 +11794,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="30">
+    <row r="8" spans="1:19" ht="28.8">
       <c r="A8" s="5" t="s">
         <v>127</v>
       </c>
@@ -11881,7 +11824,7 @@
       <c r="Q8" s="6"/>
       <c r="R8" s="5"/>
     </row>
-    <row r="9" spans="1:19" ht="30">
+    <row r="9" spans="1:19" ht="28.8">
       <c r="A9" s="5" t="s">
         <v>93</v>
       </c>
@@ -11911,7 +11854,7 @@
       <c r="Q9" s="3"/>
       <c r="R9" s="3"/>
     </row>
-    <row r="10" spans="1:19" ht="30">
+    <row r="10" spans="1:19" ht="28.8">
       <c r="A10" s="5" t="s">
         <v>95</v>
       </c>
@@ -11936,7 +11879,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="30">
+    <row r="11" spans="1:19" ht="28.8">
       <c r="A11" s="5" t="s">
         <v>96</v>
       </c>
@@ -11968,7 +11911,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" location="TestCases!B52" display="Test Description" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
+    <hyperlink ref="A1" location="TestCases!B52" display="Test Description"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -11976,7 +11919,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet19"/>
   <dimension ref="A1:E11"/>
   <sheetViews>
@@ -11984,13 +11927,13 @@
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" style="25" customWidth="1"/>
+    <col min="1" max="1" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.44140625" customWidth="1"/>
+    <col min="3" max="3" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.88671875" customWidth="1"/>
+    <col min="5" max="5" width="13.44140625" style="25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -12100,7 +12043,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Sheet20"/>
   <dimension ref="A1:H8"/>
   <sheetViews>
@@ -12108,15 +12051,15 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" customWidth="1"/>
-    <col min="2" max="2" width="30.28515625" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" customWidth="1"/>
-    <col min="5" max="6" width="16.28515625" customWidth="1"/>
+    <col min="1" max="1" width="16.44140625" customWidth="1"/>
+    <col min="2" max="2" width="30.33203125" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" customWidth="1"/>
+    <col min="4" max="4" width="11.88671875" customWidth="1"/>
+    <col min="5" max="6" width="16.33203125" customWidth="1"/>
     <col min="7" max="7" width="43" style="15" customWidth="1"/>
-    <col min="8" max="8" width="19.85546875" customWidth="1"/>
+    <col min="8" max="8" width="19.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">

</xml_diff>